<commit_message>
Update data input spreadsheet
</commit_message>
<xml_diff>
--- a/progression_estimation_input.xlsx
+++ b/progression_estimation_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholascroucher/Documents/progression_rate_estimation/progressionEstimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AADE3EE-BE8B-2E44-B7E1-EA9E5976B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECBF57D-F4A8-7D49-859A-C108365FD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="1220" windowWidth="24440" windowHeight="12540" xr2:uid="{68B6CDF4-21FC-164B-AD92-181213EE6C3E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>study</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>carriage</t>
+  </si>
+  <si>
+    <t>strain</t>
   </si>
 </sst>
 </file>
@@ -415,9 +418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC935FF1-1BCC-4F45-848F-DA69E54893DF}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -429,7 +434,7 @@
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,9 +456,12 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="study" prompt="Unique name of the case-carrier study." sqref="A1:A1048576" xr:uid="{2435CC46-B0F7-5E4E-8AD4-F163026A9A43}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="categorisation" prompt="The label of the subdivision of the microbial population" sqref="B1:B1048576" xr:uid="{76DB945B-4317-0741-A9F1-6F3EE74306A3}"/>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="carriage" prompt="The number of isolates of this subtype recovered from asymptomatic carriers (must be a non-negative integer)" sqref="C1:C1048576" xr:uid="{BAE78EC0-D7B3-1741-9D15-2E811F22465D}">
@@ -471,6 +479,7 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="time_interval" prompt="The duration of the disease surveillance period (must be consistent across each study)" sqref="G1:G1048576" xr:uid="{7D5C3DA2-22EC-F746-AB8E-DFE0F6C2EECB}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="strain" prompt="Optional column specifying the strain background when two subtyping categoriations are used in the analysis" sqref="H1:H1048576" xr:uid="{EEEAAE33-77E6-8947-BE6B-00538FD9F9CA}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change type column name
</commit_message>
<xml_diff>
--- a/progression_estimation_input.xlsx
+++ b/progression_estimation_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholascroucher/Documents/progression_rate_estimation/progressionEstimation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECBF57D-F4A8-7D49-859A-C108365FD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A442CC-163B-9246-B0E6-179F825EBAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="1220" windowWidth="24440" windowHeight="12540" xr2:uid="{68B6CDF4-21FC-164B-AD92-181213EE6C3E}"/>
+    <workbookView xWindow="-32580" yWindow="2580" windowWidth="31940" windowHeight="13280" xr2:uid="{68B6CDF4-21FC-164B-AD92-181213EE6C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="case_carriage_study" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>study</t>
   </si>
   <si>
-    <t>categorisation</t>
-  </si>
-  <si>
     <t>carriage_samples</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>strain</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,31 +439,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="study" prompt="Unique name of the case-carrier study." sqref="A1:A1048576" xr:uid="{2435CC46-B0F7-5E4E-8AD4-F163026A9A43}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="categorisation" prompt="The label of the subdivision of the microbial population" sqref="B1:B1048576" xr:uid="{76DB945B-4317-0741-A9F1-6F3EE74306A3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="type" prompt="The subdivision of the microbial population to which the isolates belong" sqref="B1:B1048576" xr:uid="{76DB945B-4317-0741-A9F1-6F3EE74306A3}"/>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="carriage" prompt="The number of isolates of this subtype recovered from asymptomatic carriers (must be a non-negative integer)" sqref="C1:C1048576" xr:uid="{BAE78EC0-D7B3-1741-9D15-2E811F22465D}">
       <formula1>0</formula1>
     </dataValidation>

</xml_diff>